<commit_message>
add file vercel.json, update report.xlsx, update app.jsx
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Báo cáo tiến độ - phân chia công việc</t>
   </si>
@@ -37,6 +37,36 @@
   </si>
   <si>
     <t xml:space="preserve"> Ngày bắt đầu</t>
+  </si>
+  <si>
+    <t>Nguyễn Thanh Huy</t>
+  </si>
+  <si>
+    <t>24/12/2023</t>
+  </si>
+  <si>
+    <t>25/11/2023</t>
+  </si>
+  <si>
+    <t>Làm page đặt vé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chức năng thêm, xóa, sửa, xem user của trang admin, pagination </t>
+  </si>
+  <si>
+    <t>Phan Vũ Công Thành</t>
+  </si>
+  <si>
+    <t>Làm chức năng đặt vé, khi chọn ghế xong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chức năng thêm, xóa, sửa, xem danh sách phim </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chức năng tạo lịch chiếu cho phim </t>
+  </si>
+  <si>
+    <t>Làm chức năng tìm kiếm user và phim</t>
   </si>
 </sst>
 </file>
@@ -74,12 +104,12 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -361,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -372,38 +402,86 @@
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
     <col min="3" max="3" width="19.77734375" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="53.77734375" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>